<commit_message>
variables codées pas en dur +  inversion arrivée et départ
</commit_message>
<xml_diff>
--- a/Data/MIS_2022_v3_aller_simple.xlsx
+++ b/Data/MIS_2022_v3_aller_simple.xlsx
@@ -1180,11 +1180,11 @@
   </sheetPr>
   <dimension ref="A1:K377"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.37"/>
@@ -1193,7 +1193,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.43"/>

</xml_diff>